<commit_message>
Added Journals, Added attendance, Modifeid Code to Save csv
</commit_message>
<xml_diff>
--- a/attendance/Spring2021_JITI_Attendance.xlsx
+++ b/attendance/Spring2021_JITI_Attendance.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="B3" s="7">
         <f>SUM(C3:M3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -566,7 +566,9 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -584,7 +586,7 @@
       </c>
       <c r="B4" s="7">
         <f t="shared" ref="B4:B8" si="2">SUM(C4:M4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -592,7 +594,9 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -610,7 +614,7 @@
       </c>
       <c r="B5" s="7">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -618,7 +622,9 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -636,7 +642,7 @@
       </c>
       <c r="B6" s="7">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -644,7 +650,9 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -662,7 +670,7 @@
       </c>
       <c r="B7" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -670,7 +678,9 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -696,7 +706,9 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -714,7 +726,7 @@
       </c>
       <c r="B9" s="7">
         <f>MAX(B3:B8)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Journals, Added attendance
</commit_message>
<xml_diff>
--- a/attendance/Spring2021_JITI_Attendance.xlsx
+++ b/attendance/Spring2021_JITI_Attendance.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="B3" s="7">
         <f>SUM(C3:M3)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -569,7 +569,9 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -586,7 +588,7 @@
       </c>
       <c r="B4" s="7">
         <f t="shared" ref="B4:B8" si="2">SUM(C4:M4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -597,7 +599,9 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -614,7 +618,7 @@
       </c>
       <c r="B5" s="7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -625,7 +629,9 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -642,7 +648,7 @@
       </c>
       <c r="B6" s="7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -653,7 +659,9 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -681,7 +689,9 @@
       <c r="E7" s="1">
         <v>1</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -698,7 +708,7 @@
       </c>
       <c r="B8" s="7">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -709,7 +719,9 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -726,7 +738,7 @@
       </c>
       <c r="B9" s="7">
         <f>MAX(B3:B8)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added recent Journal and attendance
</commit_message>
<xml_diff>
--- a/attendance/Spring2021_JITI_Attendance.xlsx
+++ b/attendance/Spring2021_JITI_Attendance.xlsx
@@ -477,7 +477,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="B3" s="7">
         <f>SUM(C3:M3)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -572,7 +572,9 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -588,7 +590,7 @@
       </c>
       <c r="B4" s="7">
         <f t="shared" ref="B4:B8" si="2">SUM(C4:M4)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -602,7 +604,9 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -618,7 +622,7 @@
       </c>
       <c r="B5" s="7">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -632,7 +636,9 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -648,7 +654,7 @@
       </c>
       <c r="B6" s="7">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -662,7 +668,9 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -678,7 +686,7 @@
       </c>
       <c r="B7" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -692,7 +700,9 @@
       <c r="F7" s="1">
         <v>0</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -708,7 +718,7 @@
       </c>
       <c r="B8" s="7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -722,7 +732,9 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -738,7 +750,7 @@
       </c>
       <c r="B9" s="7">
         <f>MAX(B3:B8)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added 2nd Presentation and Journals
</commit_message>
<xml_diff>
--- a/attendance/Spring2021_JITI_Attendance.xlsx
+++ b/attendance/Spring2021_JITI_Attendance.xlsx
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="B3" s="7">
         <f>SUM(C3:M3)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -578,9 +578,15 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -592,7 +598,7 @@
       </c>
       <c r="B4" s="7">
         <f t="shared" ref="B4:B8" si="2">SUM(C4:M4)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -612,9 +618,15 @@
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -626,7 +638,7 @@
       </c>
       <c r="B5" s="7">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -646,9 +658,15 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -660,7 +678,7 @@
       </c>
       <c r="B6" s="7">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -680,9 +698,15 @@
       <c r="H6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -694,7 +718,7 @@
       </c>
       <c r="B7" s="7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -714,9 +738,15 @@
       <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -728,7 +758,7 @@
       </c>
       <c r="B8" s="7">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -748,9 +778,15 @@
       <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -761,8 +797,8 @@
         <v>6</v>
       </c>
       <c r="B9" s="7">
-        <f>MAX(B3:B8)</f>
-        <v>6</v>
+        <f>MAX(B3:B8) -1</f>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added code to standardize the weeks and journal stubs
</commit_message>
<xml_diff>
--- a/attendance/Spring2021_JITI_Attendance.xlsx
+++ b/attendance/Spring2021_JITI_Attendance.xlsx
@@ -53,9 +53,6 @@
     <t>Aashay</t>
   </si>
   <si>
-    <t>Maximum</t>
-  </si>
-  <si>
     <t>Ania</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>Lindsey</t>
+  </si>
+  <si>
+    <t>Maximum Possible (Excluding optional meetings)</t>
   </si>
 </sst>
 </file>
@@ -474,15 +474,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" ht="52.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,7 +500,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -545,20 +548,23 @@
         <v>44300</v>
       </c>
       <c r="N2" s="4">
+        <v>44307</v>
+      </c>
+      <c r="O2" s="4">
         <v>44310</v>
       </c>
-      <c r="O2" s="4">
+      <c r="P2" s="4">
         <f>M2+14</f>
         <v>44314</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7">
-        <f>SUM(C3:M3)</f>
-        <v>9</v>
+        <f>SUM(C3:N3)</f>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -587,18 +593,25 @@
       <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="7">
-        <f t="shared" ref="B4:B8" si="2">SUM(C4:M4)</f>
-        <v>9</v>
+        <f t="shared" ref="B4:B8" si="2">SUM(C4:N4)</f>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -627,18 +640,25 @@
       <c r="K4" s="1">
         <v>1</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
       <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="7">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -667,18 +687,25 @@
       <c r="K5" s="1">
         <v>1</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
       <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="7">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -707,18 +734,25 @@
       <c r="K6" s="1">
         <v>1</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
       <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="7">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -747,18 +781,25 @@
       <c r="K7" s="1">
         <v>1</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
       <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -787,21 +828,28 @@
       <c r="K8" s="1">
         <v>1</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
       <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9" s="7">
         <f>MAX(B3:B8) -1</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C11" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added final Sub Team presentation and Attendance
</commit_message>
<xml_diff>
--- a/attendance/Spring2021_JITI_Attendance.xlsx
+++ b/attendance/Spring2021_JITI_Attendance.xlsx
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="52.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" ht="52.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -500,7 +500,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -553,18 +553,14 @@
       <c r="O2" s="4">
         <v>44310</v>
       </c>
-      <c r="P2" s="4">
-        <f>M2+14</f>
-        <v>44314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7">
-        <f>SUM(C3:N3)</f>
-        <v>12</v>
+        <f>SUM(C3:O3)</f>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -602,16 +598,17 @@
       <c r="N3" s="1">
         <v>1</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="7">
-        <f t="shared" ref="B4:B8" si="2">SUM(C4:N4)</f>
-        <v>12</v>
+        <f t="shared" ref="B4:B8" si="2">SUM(C4:O4)</f>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -649,16 +646,17 @@
       <c r="N4" s="1">
         <v>1</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="7">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -696,16 +694,17 @@
       <c r="N5" s="1">
         <v>1</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="7">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -743,16 +742,17 @@
       <c r="N6" s="1">
         <v>0</v>
       </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -790,16 +790,17 @@
       <c r="N7" s="1">
         <v>0</v>
       </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -837,19 +838,20 @@
       <c r="N8" s="1">
         <v>1</v>
       </c>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="7">
         <f>MAX(B3:B8) -1</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C11" s="6"/>
     </row>
   </sheetData>

</xml_diff>